<commit_message>
Change in licensing calculation
</commit_message>
<xml_diff>
--- a/snippets/Sentinel/M365-LogSize/M365LogSize-Estimator.xlsx
+++ b/snippets/Sentinel/M365-LogSize/M365LogSize-Estimator.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jokerit-my.sharepoint.com/personal/yannic_joker-it_ch/Documents/Kunden Temp/ZKB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\github\graber.cloud-azure-templates\snippets\Sentinel\M365-LogSize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{A1C5CD83-8641-4251-A180-DDABE23D6FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38D03768-92AF-4203-82AA-AECC2212D108}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F684A048-F6B2-4056-AB96-2C8A23DCEE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0028FBD1-AB05-4987-A241-495A07B40DC8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0028FBD1-AB05-4987-A241-495A07B40DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Defender for Endpoint</t>
   </si>
@@ -72,9 +71,6 @@
     <t>MB/d</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Fill all the blue fields. Do not change other fields</t>
   </si>
   <si>
@@ -114,15 +110,6 @@
     <t>M365 G5 Security</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>If you hold one of the following licenses, please select "yes" in the dropdown.</t>
-  </si>
-  <si>
     <t>License Benefit in MB</t>
   </si>
   <si>
@@ -136,6 +123,12 @@
   </si>
   <si>
     <t>Avg usr Billable MB/d</t>
+  </si>
+  <si>
+    <t>If you hold one of the following licenses, please insert the number of licenses for each</t>
+  </si>
+  <si>
+    <t>(only licensed users count)</t>
   </si>
 </sst>
 </file>
@@ -473,6 +466,82 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -508,82 +577,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="0"/>
@@ -648,30 +641,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4184E8B3-B97F-4DB4-AB21-A7DFA1E9BD60}" name="Table3" displayName="Table3" ref="A7:F13" totalsRowCount="1" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="A7:F12" xr:uid="{4184E8B3-B97F-4DB4-AB21-A7DFA1E9BD60}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB27CF67-CD2F-461E-A798-4925C4AD36F4}" name=" " totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E8E44035-F124-43C0-99B7-90199BF999F6}" name="Count" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B06F6AC0-9188-4E54-92DF-3BA985CE1A06}" name="MB" dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{AB27CF67-CD2F-461E-A798-4925C4AD36F4}" name=" " totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{E8E44035-F124-43C0-99B7-90199BF999F6}" name="Count" dataDxfId="10" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{B06F6AC0-9188-4E54-92DF-3BA985CE1A06}" name="MB" dataDxfId="9" totalsRowDxfId="3"/>
     <tableColumn id="4" xr3:uid="{A0B3BBA9-888E-4A42-A505-F201C286781E}" name="MB/d" dataDxfId="8" totalsRowDxfId="2">
       <calculatedColumnFormula>C8/730*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9B781895-20A6-451E-A61B-180C51DBE6A8}" name="GB/d" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="1">
+    <tableColumn id="5" xr3:uid="{9B781895-20A6-451E-A61B-180C51DBE6A8}" name="GB/d" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="1">
       <calculatedColumnFormula>D8/1024</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6B360999-3095-4C40-A497-D9D084DDC6FE}" name="avg usr MB/d" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0">
+    <tableColumn id="6" xr3:uid="{6B360999-3095-4C40-A497-D9D084DDC6FE}" name="avg usr MB/d" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="0">
       <calculatedColumnFormula>D8/$B$5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35A60AA4-1290-446C-B561-6D5A48FA3C1D}" name="Table1" displayName="Table1" ref="A1:A3" totalsRowShown="0">
-  <autoFilter ref="A1:A3" xr:uid="{35A60AA4-1290-446C-B561-6D5A48FA3C1D}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{09F638F3-AC92-4748-A180-7D91169E9143}" name="Column1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -992,38 +975,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7864BCA4-56C4-4496-B2B8-6BBF72B5F00D}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -1031,10 +1014,10 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1049,105 +1032,125 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3">
+        <v>541458498</v>
+      </c>
+      <c r="C8" s="3">
+        <v>486359.75</v>
+      </c>
       <c r="D8" s="6">
         <f>C8/730*24</f>
-        <v>0</v>
+        <v>15989.909589041097</v>
       </c>
       <c r="E8" s="6">
         <f>D8/1024</f>
-        <v>0</v>
+        <v>15.615146083047946</v>
       </c>
       <c r="F8" s="6">
         <f t="shared" ref="F8:F12" si="0">D8/$B$5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6.3959638356164392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3">
+        <v>12496671</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4397.0200000000004</v>
+      </c>
       <c r="D9" s="6">
         <f t="shared" ref="D9:D12" si="1">C9/730*24</f>
-        <v>0</v>
+        <v>144.55956164383562</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" ref="E9:E12" si="2">D9/1024</f>
-        <v>0</v>
+        <v>0.14117144691780822</v>
       </c>
       <c r="F9" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5.7823824657534252E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3">
+        <v>11534952</v>
+      </c>
+      <c r="C10" s="3">
+        <v>23771.32</v>
+      </c>
       <c r="D10" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>781.52284931506847</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.76320590753424655</v>
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.31260913972602739</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3">
+        <v>16119836</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9387.42</v>
+      </c>
       <c r="D11" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>308.62750684931507</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.30139404965753425</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.12345100273972602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3">
+        <v>25689</v>
+      </c>
+      <c r="C12" s="3">
+        <v>41.9</v>
+      </c>
       <c r="D12" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.3775342465753424</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.3452482876712328E-3</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>5.5101369863013697E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1156,16 +1159,16 @@
       <c r="D13" s="7"/>
       <c r="E13" s="11">
         <f>SUBTOTAL(109,Table3[GB/d])</f>
-        <v>0</v>
+        <v>16.822262735445207</v>
       </c>
       <c r="F13" s="11">
         <f>SUBTOTAL(109,Table3[avg usr MB/d])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6.8903988164383572</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -1173,169 +1176,137 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17">
+        <f>Table3[[#Totals],[avg usr MB/d]]</f>
+        <v>6.8903988164383572</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="19">
+        <f>B17*5+B18*5+B19*5+B20*5+B21*5+B22*5+B23*5+B24*5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="18">
+        <f>B26-IF(B27=0,0,5)</f>
+        <v>6.8903988164383572</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="16">
+        <f>B26*B5-B27</f>
+        <v>17225.997041095892</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="17">
-        <f>Table3[[#Totals],[avg usr MB/d]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="19">
-        <f>IF(B16="no",IF(B17="no",IF(B18="no",IF(B19="no",IF(B20="no",IF(B21="no",IF(B22="no",IF(B23="no",0,5*B5),5*B5),5*B5),5*B5),5*B5),5*B5),5*B5),5*B5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="18">
-        <f>B25-IF(B26=0,0,5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="16">
-        <f>B25*B5-B26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="16">
-        <f>B28/1024</f>
-        <v>0</v>
+      <c r="B30" s="16">
+        <f>B29/1024</f>
+        <v>16.822262735445207</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B24" xr:uid="{48EA67F8-0138-4514-9762-CC52ADC5285B}">
+      <formula1>0</formula1>
+      <formula2>1000000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{48EA67F8-0138-4514-9762-CC52ADC5285B}">
-          <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B16:B23</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89DB0DED-1261-4527-AD64-521C5F5E8852}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>